<commit_message>
Excel Column names done
</commit_message>
<xml_diff>
--- a/ExpenseReport.xlsx
+++ b/ExpenseReport.xlsx
@@ -424,48 +424,48 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Travel</t>
+          <t>Date</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>1500.00</t>
+          <t>Total Amount</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Public</t>
+          <t>2023-06-18</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>43.00</t>
+          <t>2387.00</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Rents</t>
+          <t>2023-06-06</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>784.00</t>
+          <t>213.00</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Fruits</t>
+          <t>2023-06-15</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>273.00</t>
+          <t>50.00</t>
         </is>
       </c>
     </row>

</xml_diff>